<commit_message>
remove unused code, add comments
</commit_message>
<xml_diff>
--- a/stepbystep.xlsx
+++ b/stepbystep.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/Library/CloudStorage/iCloud Drive/Documents/Summer/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD69356-35F6-CD4D-80D5-7D67118475E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC489622-1F3F-1442-A8D9-97A04F89CBBA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1180" windowWidth="25440" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="1180" windowWidth="25440" windowHeight="16780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species" sheetId="1" r:id="rId1"/>
     <sheet name="reactions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -164,7 +165,7 @@
     <t>Ras family of GTPases</t>
   </si>
   <si>
-    <t>FPR1 =&gt; Sos</t>
+    <t>FPR1 ===&gt; Sos</t>
   </si>
 </sst>
 </file>
@@ -715,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DK33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1736,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AY123"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>